<commit_message>
updated templaet (added GB)
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">MATERIALBERICHT</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Datenmenge Bild:     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
   </si>
   <si>
     <t xml:space="preserve">Kopierer:</t>
@@ -359,9 +362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>363240</xdr:colOff>
+      <xdr:colOff>362880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -375,7 +378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9661320" cy="1244160"/>
+          <a:ext cx="9666720" cy="1243800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -397,17 +400,17 @@
   </sheetPr>
   <dimension ref="C10:M59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M54" activeCellId="0" sqref="M54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.54"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,21 +529,27 @@
         <v>21</v>
       </c>
       <c r="K53" s="4"/>
+      <c r="M53" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K54" s="4"/>
+      <c r="M54" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="4"/>
@@ -550,10 +559,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -572,13 +584,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="11" t="n">

</xml_diff>